<commit_message>
Basic virheenkäsittelyä, täytynee jatkaa vielä
</commit_message>
<xml_diff>
--- a/Harjoitustyö_Ryhmä5_Jeff/Data/Toimittajarekisteri.xlsx
+++ b/Harjoitustyö_Ryhmä5_Jeff/Data/Toimittajarekisteri.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ad193d0551a0b3/Asiakirjat/GitHub/UiPath_Jeff/Harjoitustyö_Ryhmä5_Jeff/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valtteri.000\Documents\UiPath\Jeff\Harjoitustyö_Ryhmä5_Jeff\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{C8F535F1-D860-498C-B71A-D55245652788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941CA96A-5157-4F6D-9809-D394CA33C19D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E67AE8-6CA5-4D56-A6E8-BCEF78A78026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2507" yWindow="0" windowWidth="17493" windowHeight="12613" xr2:uid="{F0EDB271-B87F-4FD9-8480-9C455521B989}"/>
+    <workbookView xWindow="2280" yWindow="2895" windowWidth="20790" windowHeight="11625" xr2:uid="{F0EDB271-B87F-4FD9-8480-9C455521B989}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,68 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Toimittajanro</t>
+  </si>
+  <si>
+    <t>Y-Tunnus</t>
+  </si>
+  <si>
+    <t>Toimittaja</t>
+  </si>
+  <si>
+    <t>Summa</t>
+  </si>
+  <si>
+    <t>Osoite</t>
+  </si>
+  <si>
+    <t>Postinumero</t>
+  </si>
+  <si>
+    <t>Kaupunki</t>
+  </si>
+  <si>
+    <t>Tilinro</t>
+  </si>
+  <si>
+    <t>Pankki</t>
+  </si>
+  <si>
+    <t>0725937-3</t>
+  </si>
+  <si>
+    <t>E-K SOSIAALI- JA TERVEYSPIIRI</t>
+  </si>
+  <si>
+    <t>2977551-2</t>
+  </si>
+  <si>
+    <t>PEAB INDUSTRI OY</t>
+  </si>
+  <si>
+    <t>2752472-8</t>
+  </si>
+  <si>
+    <t>PALLAS RAKENNUS KAAKKOIS-SUOMI</t>
+  </si>
+  <si>
+    <t>0162017-2</t>
+  </si>
+  <si>
+    <t>SAIMAAN TUKIPALVELUT OY</t>
+  </si>
+  <si>
+    <t>1565583-5</t>
+  </si>
+  <si>
+    <t>YIT SUOMI OY</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,14 +443,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1A0006-AF6A-4106-8A0D-947B7BA43FF6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>21509717.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>73978</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>860908.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>77161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>782500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38975</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>560267.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>67122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>400000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>